<commit_message>
adjust u dist funciton bakeup v1.0.4
</commit_message>
<xml_diff>
--- a/raws/SmartVIP_生产检测_工程文件/20170703_JL207A_生产检测_总检测试.xlsx
+++ b/raws/SmartVIP_生产检测_工程文件/20170703_JL207A_生产检测_总检测试.xlsx
@@ -674,15 +674,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0000=江铃福特、0001=一汽解、0002=通用客户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0x00=SHORT、0x01=OK、0x02=OPEN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>0x00=正常、0x01=欠压/无电池</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000=江铃福特、0001=一汽解放、0002=通用客户</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1244,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2031,7 +2031,7 @@
         <v>13</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>47</v>
@@ -2060,7 +2060,7 @@
         <v>13</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>46</v>
@@ -2408,7 +2408,7 @@
         <v>13</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>46</v>

</xml_diff>